<commit_message>
Add functionality to read information about individual wells
</commit_message>
<xml_diff>
--- a/cytation_5_plate2.xlsx
+++ b/cytation_5_plate2.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gerald\Desktop\School Stuff\Sem 7\FYP\EBase + PBase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEEADB7F-D825-407B-B37D-7B05291EC0DD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB4AE10-671B-4CE8-A587-824BD609D26C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Metadata" sheetId="2" r:id="rId2"/>
+    <sheet name="Well Information" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="MethodPointer1">-13108848</definedName>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="178">
   <si>
     <t>Software Version</t>
   </si>
@@ -723,6 +724,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -732,7 +734,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -31535,7 +31536,7 @@
       </c>
     </row>
     <row r="160" spans="1:99" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B160" s="15" t="s">
+      <c r="B160" s="16" t="s">
         <v>147</v>
       </c>
       <c r="C160" s="9">
@@ -31579,7 +31580,7 @@
       </c>
     </row>
     <row r="161" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B161" s="16"/>
+      <c r="B161" s="17"/>
       <c r="C161" s="11">
         <v>1</v>
       </c>
@@ -31621,7 +31622,7 @@
       </c>
     </row>
     <row r="162" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B162" s="16"/>
+      <c r="B162" s="17"/>
       <c r="C162" s="12">
         <v>0.1909490740740741</v>
       </c>
@@ -31663,7 +31664,7 @@
       </c>
     </row>
     <row r="163" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B163" s="16"/>
+      <c r="B163" s="17"/>
       <c r="C163" s="12">
         <v>0.10831018518518519</v>
       </c>
@@ -31705,7 +31706,7 @@
       </c>
     </row>
     <row r="164" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B164" s="16"/>
+      <c r="B164" s="17"/>
       <c r="C164" s="11">
         <v>-54200</v>
       </c>
@@ -31747,7 +31748,7 @@
       </c>
     </row>
     <row r="165" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B165" s="16"/>
+      <c r="B165" s="17"/>
       <c r="C165" s="11">
         <v>1</v>
       </c>
@@ -31789,7 +31790,7 @@
       </c>
     </row>
     <row r="166" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B166" s="16"/>
+      <c r="B166" s="17"/>
       <c r="C166" s="12">
         <v>1.4456018518518519E-2</v>
       </c>
@@ -31831,7 +31832,7 @@
       </c>
     </row>
     <row r="167" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B167" s="16"/>
+      <c r="B167" s="17"/>
       <c r="C167" s="12">
         <v>9.2476851851851852E-3</v>
       </c>
@@ -31873,7 +31874,7 @@
       </c>
     </row>
     <row r="168" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B168" s="16"/>
+      <c r="B168" s="17"/>
       <c r="C168" s="11">
         <v>333.33300000000003</v>
       </c>
@@ -31915,7 +31916,7 @@
       </c>
     </row>
     <row r="169" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B169" s="16"/>
+      <c r="B169" s="17"/>
       <c r="C169" s="11">
         <v>1</v>
       </c>
@@ -31957,7 +31958,7 @@
       </c>
     </row>
     <row r="170" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B170" s="16"/>
+      <c r="B170" s="17"/>
       <c r="C170" s="12">
         <v>5.6689814814814811E-2</v>
       </c>
@@ -31999,7 +32000,7 @@
       </c>
     </row>
     <row r="171" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B171" s="17"/>
+      <c r="B171" s="18"/>
       <c r="C171" s="13">
         <v>4.731481481481481E-2</v>
       </c>
@@ -32041,7 +32042,7 @@
       </c>
     </row>
     <row r="172" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B172" s="15" t="s">
+      <c r="B172" s="16" t="s">
         <v>160</v>
       </c>
       <c r="C172" s="9">
@@ -32085,7 +32086,7 @@
       </c>
     </row>
     <row r="173" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B173" s="16"/>
+      <c r="B173" s="17"/>
       <c r="C173" s="11">
         <v>1</v>
       </c>
@@ -32127,7 +32128,7 @@
       </c>
     </row>
     <row r="174" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B174" s="16"/>
+      <c r="B174" s="17"/>
       <c r="C174" s="12">
         <v>0.13886574074074073</v>
       </c>
@@ -32169,7 +32170,7 @@
       </c>
     </row>
     <row r="175" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B175" s="16"/>
+      <c r="B175" s="17"/>
       <c r="C175" s="12">
         <v>0.10016203703703704</v>
       </c>
@@ -32211,7 +32212,7 @@
       </c>
     </row>
     <row r="176" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B176" s="16"/>
+      <c r="B176" s="17"/>
       <c r="C176" s="11">
         <v>-64400</v>
       </c>
@@ -32253,7 +32254,7 @@
       </c>
     </row>
     <row r="177" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B177" s="16"/>
+      <c r="B177" s="17"/>
       <c r="C177" s="11">
         <v>1</v>
       </c>
@@ -32295,7 +32296,7 @@
       </c>
     </row>
     <row r="178" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B178" s="16"/>
+      <c r="B178" s="17"/>
       <c r="C178" s="12">
         <v>1.4456018518518519E-2</v>
       </c>
@@ -32337,7 +32338,7 @@
       </c>
     </row>
     <row r="179" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B179" s="16"/>
+      <c r="B179" s="17"/>
       <c r="C179" s="12">
         <v>9.2476851851851852E-3</v>
       </c>
@@ -32379,7 +32380,7 @@
       </c>
     </row>
     <row r="180" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B180" s="16"/>
+      <c r="B180" s="17"/>
       <c r="C180" s="11">
         <v>-466.66699999999997</v>
       </c>
@@ -32421,7 +32422,7 @@
       </c>
     </row>
     <row r="181" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B181" s="16"/>
+      <c r="B181" s="17"/>
       <c r="C181" s="11">
         <v>1</v>
       </c>
@@ -32463,7 +32464,7 @@
       </c>
     </row>
     <row r="182" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B182" s="16"/>
+      <c r="B182" s="17"/>
       <c r="C182" s="12">
         <v>4.6273148148148147E-2</v>
       </c>
@@ -32505,7 +32506,7 @@
       </c>
     </row>
     <row r="183" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B183" s="17"/>
+      <c r="B183" s="18"/>
       <c r="C183" s="13">
         <v>4.553240740740741E-2</v>
       </c>
@@ -32547,7 +32548,7 @@
       </c>
     </row>
     <row r="184" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B184" s="15" t="s">
+      <c r="B184" s="16" t="s">
         <v>161</v>
       </c>
       <c r="C184" s="9">
@@ -32591,7 +32592,7 @@
       </c>
     </row>
     <row r="185" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B185" s="16"/>
+      <c r="B185" s="17"/>
       <c r="C185" s="11">
         <v>1</v>
       </c>
@@ -32633,7 +32634,7 @@
       </c>
     </row>
     <row r="186" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B186" s="16"/>
+      <c r="B186" s="17"/>
       <c r="C186" s="12">
         <v>0.13886574074074073</v>
       </c>
@@ -32675,7 +32676,7 @@
       </c>
     </row>
     <row r="187" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B187" s="16"/>
+      <c r="B187" s="17"/>
       <c r="C187" s="12">
         <v>8.6168981481481485E-2</v>
       </c>
@@ -32717,7 +32718,7 @@
       </c>
     </row>
     <row r="188" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B188" s="16"/>
+      <c r="B188" s="17"/>
       <c r="C188" s="11">
         <v>-47066.667000000001</v>
       </c>
@@ -32759,7 +32760,7 @@
       </c>
     </row>
     <row r="189" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B189" s="16"/>
+      <c r="B189" s="17"/>
       <c r="C189" s="11">
         <v>1</v>
       </c>
@@ -32801,7 +32802,7 @@
       </c>
     </row>
     <row r="190" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B190" s="16"/>
+      <c r="B190" s="17"/>
       <c r="C190" s="12">
         <v>1.4456018518518519E-2</v>
       </c>
@@ -32843,7 +32844,7 @@
       </c>
     </row>
     <row r="191" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B191" s="16"/>
+      <c r="B191" s="17"/>
       <c r="C191" s="12">
         <v>9.2476851851851852E-3</v>
       </c>
@@ -32885,7 +32886,7 @@
       </c>
     </row>
     <row r="192" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B192" s="16"/>
+      <c r="B192" s="17"/>
       <c r="C192" s="11">
         <v>333.33300000000003</v>
       </c>
@@ -32927,7 +32928,7 @@
       </c>
     </row>
     <row r="193" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B193" s="16"/>
+      <c r="B193" s="17"/>
       <c r="C193" s="11">
         <v>1</v>
       </c>
@@ -32969,7 +32970,7 @@
       </c>
     </row>
     <row r="194" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B194" s="16"/>
+      <c r="B194" s="17"/>
       <c r="C194" s="12">
         <v>4.6273148148148147E-2</v>
       </c>
@@ -33011,7 +33012,7 @@
       </c>
     </row>
     <row r="195" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B195" s="17"/>
+      <c r="B195" s="18"/>
       <c r="C195" s="13">
         <v>4.3148148148148151E-2</v>
       </c>
@@ -33053,7 +33054,7 @@
       </c>
     </row>
     <row r="196" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B196" s="15" t="s">
+      <c r="B196" s="16" t="s">
         <v>162</v>
       </c>
       <c r="C196" s="9">
@@ -33097,7 +33098,7 @@
       </c>
     </row>
     <row r="197" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B197" s="16"/>
+      <c r="B197" s="17"/>
       <c r="C197" s="11">
         <v>1</v>
       </c>
@@ -33139,7 +33140,7 @@
       </c>
     </row>
     <row r="198" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B198" s="16"/>
+      <c r="B198" s="17"/>
       <c r="C198" s="12">
         <v>0.28469907407407408</v>
       </c>
@@ -33181,7 +33182,7 @@
       </c>
     </row>
     <row r="199" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B199" s="16"/>
+      <c r="B199" s="17"/>
       <c r="C199" s="12">
         <v>0.16064814814814815</v>
       </c>
@@ -33223,7 +33224,7 @@
       </c>
     </row>
     <row r="200" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B200" s="16"/>
+      <c r="B200" s="17"/>
       <c r="C200" s="11">
         <v>98933.332999999999</v>
       </c>
@@ -33265,7 +33266,7 @@
       </c>
     </row>
     <row r="201" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B201" s="16"/>
+      <c r="B201" s="17"/>
       <c r="C201" s="11">
         <v>1</v>
       </c>
@@ -33307,7 +33308,7 @@
       </c>
     </row>
     <row r="202" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B202" s="16"/>
+      <c r="B202" s="17"/>
       <c r="C202" s="12">
         <v>4.5706018518518521E-2</v>
       </c>
@@ -33349,7 +33350,7 @@
       </c>
     </row>
     <row r="203" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B203" s="16"/>
+      <c r="B203" s="17"/>
       <c r="C203" s="12">
         <v>2.642361111111111E-2</v>
       </c>
@@ -33391,7 +33392,7 @@
       </c>
     </row>
     <row r="204" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B204" s="16"/>
+      <c r="B204" s="17"/>
       <c r="C204" s="11">
         <v>666.66700000000003</v>
       </c>
@@ -33433,7 +33434,7 @@
       </c>
     </row>
     <row r="205" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B205" s="16"/>
+      <c r="B205" s="17"/>
       <c r="C205" s="11">
         <v>1</v>
       </c>
@@ -33475,7 +33476,7 @@
       </c>
     </row>
     <row r="206" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B206" s="16"/>
+      <c r="B206" s="17"/>
       <c r="C206" s="12">
         <v>0.11918981481481482</v>
       </c>
@@ -33517,7 +33518,7 @@
       </c>
     </row>
     <row r="207" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B207" s="17"/>
+      <c r="B207" s="18"/>
       <c r="C207" s="13">
         <v>0.10981481481481481</v>
       </c>
@@ -33559,7 +33560,7 @@
       </c>
     </row>
     <row r="208" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B208" s="15" t="s">
+      <c r="B208" s="16" t="s">
         <v>164</v>
       </c>
       <c r="C208" s="9">
@@ -33603,7 +33604,7 @@
       </c>
     </row>
     <row r="209" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B209" s="16"/>
+      <c r="B209" s="17"/>
       <c r="C209" s="11">
         <v>1</v>
       </c>
@@ -33645,7 +33646,7 @@
       </c>
     </row>
     <row r="210" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B210" s="16"/>
+      <c r="B210" s="17"/>
       <c r="C210" s="12">
         <v>0.29511574074074071</v>
       </c>
@@ -33687,7 +33688,7 @@
       </c>
     </row>
     <row r="211" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B211" s="16"/>
+      <c r="B211" s="17"/>
       <c r="C211" s="12">
         <v>0.19413194444444445</v>
       </c>
@@ -33729,7 +33730,7 @@
       </c>
     </row>
     <row r="212" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B212" s="16"/>
+      <c r="B212" s="17"/>
       <c r="C212" s="11">
         <v>84866.667000000001</v>
       </c>
@@ -33771,7 +33772,7 @@
       </c>
     </row>
     <row r="213" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B213" s="16"/>
+      <c r="B213" s="17"/>
       <c r="C213" s="11">
         <v>1</v>
       </c>
@@ -33813,7 +33814,7 @@
       </c>
     </row>
     <row r="214" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B214" s="16"/>
+      <c r="B214" s="17"/>
       <c r="C214" s="12">
         <v>5.6122685185185185E-2</v>
       </c>
@@ -33855,7 +33856,7 @@
       </c>
     </row>
     <row r="215" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B215" s="16"/>
+      <c r="B215" s="17"/>
       <c r="C215" s="12">
         <v>2.8113425925925927E-2</v>
       </c>
@@ -33897,7 +33898,7 @@
       </c>
     </row>
     <row r="216" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B216" s="16"/>
+      <c r="B216" s="17"/>
       <c r="C216" s="11">
         <v>400</v>
       </c>
@@ -33939,7 +33940,7 @@
       </c>
     </row>
     <row r="217" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B217" s="16"/>
+      <c r="B217" s="17"/>
       <c r="C217" s="11">
         <v>1</v>
       </c>
@@ -33981,7 +33982,7 @@
       </c>
     </row>
     <row r="218" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B218" s="16"/>
+      <c r="B218" s="17"/>
       <c r="C218" s="12">
         <v>3.5856481481481482E-2</v>
       </c>
@@ -34023,7 +34024,7 @@
       </c>
     </row>
     <row r="219" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B219" s="17"/>
+      <c r="B219" s="18"/>
       <c r="C219" s="13">
         <v>3.7592592592592594E-2</v>
       </c>
@@ -34065,7 +34066,7 @@
       </c>
     </row>
     <row r="220" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B220" s="15" t="s">
+      <c r="B220" s="16" t="s">
         <v>165</v>
       </c>
       <c r="C220" s="9">
@@ -34109,7 +34110,7 @@
       </c>
     </row>
     <row r="221" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B221" s="16"/>
+      <c r="B221" s="17"/>
       <c r="C221" s="11">
         <v>1</v>
       </c>
@@ -34151,7 +34152,7 @@
       </c>
     </row>
     <row r="222" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B222" s="16"/>
+      <c r="B222" s="17"/>
       <c r="C222" s="12">
         <v>0.31594907407407408</v>
       </c>
@@ -34193,7 +34194,7 @@
       </c>
     </row>
     <row r="223" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B223" s="16"/>
+      <c r="B223" s="17"/>
       <c r="C223" s="12">
         <v>0.19799768518518521</v>
       </c>
@@ -34235,7 +34236,7 @@
       </c>
     </row>
     <row r="224" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B224" s="16"/>
+      <c r="B224" s="17"/>
       <c r="C224" s="11">
         <v>85266.667000000001</v>
       </c>
@@ -34277,7 +34278,7 @@
       </c>
     </row>
     <row r="225" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B225" s="16"/>
+      <c r="B225" s="17"/>
       <c r="C225" s="11">
         <v>1</v>
       </c>
@@ -34319,7 +34320,7 @@
       </c>
     </row>
     <row r="226" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B226" s="16"/>
+      <c r="B226" s="17"/>
       <c r="C226" s="12">
         <v>5.6122685185185185E-2</v>
       </c>
@@ -34361,7 +34362,7 @@
       </c>
     </row>
     <row r="227" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B227" s="16"/>
+      <c r="B227" s="17"/>
       <c r="C227" s="12">
         <v>2.8784722222222225E-2</v>
       </c>
@@ -34403,7 +34404,7 @@
       </c>
     </row>
     <row r="228" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B228" s="16"/>
+      <c r="B228" s="17"/>
       <c r="C228" s="11">
         <v>-533.33299999999997</v>
       </c>
@@ -34445,7 +34446,7 @@
       </c>
     </row>
     <row r="229" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B229" s="16"/>
+      <c r="B229" s="17"/>
       <c r="C229" s="11">
         <v>1</v>
       </c>
@@ -34487,7 +34488,7 @@
       </c>
     </row>
     <row r="230" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B230" s="16"/>
+      <c r="B230" s="17"/>
       <c r="C230" s="12">
         <v>0.26502314814814815</v>
       </c>
@@ -34529,7 +34530,7 @@
       </c>
     </row>
     <row r="231" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B231" s="17"/>
+      <c r="B231" s="18"/>
       <c r="C231" s="13">
         <v>0.27674768518518517</v>
       </c>
@@ -34571,7 +34572,7 @@
       </c>
     </row>
     <row r="232" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B232" s="15" t="s">
+      <c r="B232" s="16" t="s">
         <v>166</v>
       </c>
       <c r="C232" s="9">
@@ -34615,7 +34616,7 @@
       </c>
     </row>
     <row r="233" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B233" s="16"/>
+      <c r="B233" s="17"/>
       <c r="C233" s="11">
         <v>1</v>
       </c>
@@ -34657,7 +34658,7 @@
       </c>
     </row>
     <row r="234" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B234" s="16"/>
+      <c r="B234" s="17"/>
       <c r="C234" s="12">
         <v>2.4282407407407409E-2</v>
       </c>
@@ -34699,7 +34700,7 @@
       </c>
     </row>
     <row r="235" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B235" s="16"/>
+      <c r="B235" s="17"/>
       <c r="C235" s="12">
         <v>2.4282407407407409E-2</v>
       </c>
@@ -34741,7 +34742,7 @@
       </c>
     </row>
     <row r="236" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B236" s="16"/>
+      <c r="B236" s="17"/>
       <c r="C236" s="11">
         <v>1200</v>
       </c>
@@ -34783,7 +34784,7 @@
       </c>
     </row>
     <row r="237" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B237" s="16"/>
+      <c r="B237" s="17"/>
       <c r="C237" s="11">
         <v>1</v>
       </c>
@@ -34825,7 +34826,7 @@
       </c>
     </row>
     <row r="238" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B238" s="16"/>
+      <c r="B238" s="17"/>
       <c r="C238" s="12">
         <v>7.6956018518518521E-2</v>
       </c>
@@ -34867,7 +34868,7 @@
       </c>
     </row>
     <row r="239" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B239" s="16"/>
+      <c r="B239" s="17"/>
       <c r="C239" s="12">
         <v>8.5057870370370367E-2</v>
       </c>
@@ -34909,7 +34910,7 @@
       </c>
     </row>
     <row r="240" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B240" s="16"/>
+      <c r="B240" s="17"/>
       <c r="C240" s="11">
         <v>466.66699999999997</v>
       </c>
@@ -34951,7 +34952,7 @@
       </c>
     </row>
     <row r="241" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B241" s="16"/>
+      <c r="B241" s="17"/>
       <c r="C241" s="11">
         <v>1</v>
       </c>
@@ -34993,7 +34994,7 @@
       </c>
     </row>
     <row r="242" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B242" s="16"/>
+      <c r="B242" s="17"/>
       <c r="C242" s="12">
         <v>0.19210648148148146</v>
       </c>
@@ -35035,7 +35036,7 @@
       </c>
     </row>
     <row r="243" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B243" s="17"/>
+      <c r="B243" s="18"/>
       <c r="C243" s="13">
         <v>0.19284722222222225</v>
       </c>
@@ -35077,7 +35078,7 @@
       </c>
     </row>
     <row r="244" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B244" s="15" t="s">
+      <c r="B244" s="16" t="s">
         <v>167</v>
       </c>
       <c r="C244" s="9">
@@ -35121,7 +35122,7 @@
       </c>
     </row>
     <row r="245" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B245" s="16"/>
+      <c r="B245" s="17"/>
       <c r="C245" s="11">
         <v>1</v>
       </c>
@@ -35163,7 +35164,7 @@
       </c>
     </row>
     <row r="246" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B246" s="16"/>
+      <c r="B246" s="17"/>
       <c r="C246" s="12">
         <v>1.3865740740740739E-2</v>
       </c>
@@ -35205,7 +35206,7 @@
       </c>
     </row>
     <row r="247" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B247" s="16"/>
+      <c r="B247" s="17"/>
       <c r="C247" s="12">
         <v>8.6574074074074071E-3</v>
       </c>
@@ -35247,7 +35248,7 @@
       </c>
     </row>
     <row r="248" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B248" s="16"/>
+      <c r="B248" s="17"/>
       <c r="C248" s="11">
         <v>-6733.3329999999996</v>
       </c>
@@ -35289,7 +35290,7 @@
       </c>
     </row>
     <row r="249" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B249" s="16"/>
+      <c r="B249" s="17"/>
       <c r="C249" s="11">
         <v>1</v>
       </c>
@@ -35331,7 +35332,7 @@
       </c>
     </row>
     <row r="250" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B250" s="16"/>
+      <c r="B250" s="17"/>
       <c r="C250" s="12">
         <v>2.4872685185185189E-2</v>
       </c>
@@ -35373,7 +35374,7 @@
       </c>
     </row>
     <row r="251" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B251" s="16"/>
+      <c r="B251" s="17"/>
       <c r="C251" s="12">
         <v>1.0590277777777777E-2</v>
       </c>
@@ -35415,7 +35416,7 @@
       </c>
     </row>
     <row r="252" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B252" s="16"/>
+      <c r="B252" s="17"/>
       <c r="C252" s="11">
         <v>-1133.3330000000001</v>
       </c>
@@ -35457,7 +35458,7 @@
       </c>
     </row>
     <row r="253" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B253" s="16"/>
+      <c r="B253" s="17"/>
       <c r="C253" s="11">
         <v>1</v>
       </c>
@@ -35499,7 +35500,7 @@
       </c>
     </row>
     <row r="254" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B254" s="16"/>
+      <c r="B254" s="17"/>
       <c r="C254" s="12">
         <v>0.25460648148148152</v>
       </c>
@@ -35541,7 +35542,7 @@
       </c>
     </row>
     <row r="255" spans="2:15" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="B255" s="17"/>
+      <c r="B255" s="18"/>
       <c r="C255" s="13">
         <v>0.26165509259259262</v>
       </c>
@@ -35604,29 +35605,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B44F3C54-503F-4D08-8931-8FECD0AE1874}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>173</v>
       </c>
     </row>
@@ -35648,6 +35649,601 @@
       </c>
       <c r="F2" t="s">
         <v>174</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{020816F2-508F-4BCF-A39D-F5E262CE7465}">
+  <dimension ref="A1:CR2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R10" sqref="R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="S1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="U1" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="V1" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="W1" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="X1" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z1" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA1" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB1" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF1" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG1" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH1" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI1" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="AJ1" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="AK1" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL1" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="AO1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AQ1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="AR1" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="AS1" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="AT1" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="AU1" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="AV1" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="AW1" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="AY1" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="AZ1" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="BA1" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="BB1" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="BC1" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="BD1" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="BE1" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="BF1" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="BG1" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="BH1" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="BI1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="BJ1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="BO1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="BP1" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="BQ1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="BR1" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="BS1" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="BT1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="BU1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="BV1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="BW1" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="BX1" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="BY1" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="BZ1" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="CA1" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="CB1" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="CC1" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="CD1" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="CE1" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="CF1" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="CG1" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="CH1" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="CI1" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="CJ1" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="CK1" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="CL1" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="CM1" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="CN1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="CO1" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="CP1" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="CQ1" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="CR1" s="5" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="2" spans="1:96" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>3</v>
+      </c>
+      <c r="D2">
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>6</v>
+      </c>
+      <c r="G2">
+        <v>7</v>
+      </c>
+      <c r="H2">
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <v>9</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
+      </c>
+      <c r="K2">
+        <v>11</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>13</v>
+      </c>
+      <c r="N2">
+        <v>14</v>
+      </c>
+      <c r="O2">
+        <v>15</v>
+      </c>
+      <c r="P2">
+        <v>16</v>
+      </c>
+      <c r="Q2">
+        <v>17</v>
+      </c>
+      <c r="R2">
+        <v>18</v>
+      </c>
+      <c r="S2">
+        <v>19</v>
+      </c>
+      <c r="T2">
+        <v>20</v>
+      </c>
+      <c r="U2">
+        <v>21</v>
+      </c>
+      <c r="V2">
+        <v>22</v>
+      </c>
+      <c r="W2">
+        <v>23</v>
+      </c>
+      <c r="X2">
+        <v>24</v>
+      </c>
+      <c r="Y2">
+        <v>25</v>
+      </c>
+      <c r="Z2">
+        <v>26</v>
+      </c>
+      <c r="AA2">
+        <v>27</v>
+      </c>
+      <c r="AB2">
+        <v>28</v>
+      </c>
+      <c r="AC2">
+        <v>29</v>
+      </c>
+      <c r="AD2">
+        <v>30</v>
+      </c>
+      <c r="AE2">
+        <v>31</v>
+      </c>
+      <c r="AF2">
+        <v>32</v>
+      </c>
+      <c r="AG2">
+        <v>33</v>
+      </c>
+      <c r="AH2">
+        <v>34</v>
+      </c>
+      <c r="AI2">
+        <v>35</v>
+      </c>
+      <c r="AJ2">
+        <v>36</v>
+      </c>
+      <c r="AK2">
+        <v>37</v>
+      </c>
+      <c r="AL2">
+        <v>38</v>
+      </c>
+      <c r="AM2">
+        <v>39</v>
+      </c>
+      <c r="AN2">
+        <v>40</v>
+      </c>
+      <c r="AO2">
+        <v>41</v>
+      </c>
+      <c r="AP2">
+        <v>42</v>
+      </c>
+      <c r="AQ2">
+        <v>43</v>
+      </c>
+      <c r="AR2">
+        <v>44</v>
+      </c>
+      <c r="AS2">
+        <v>45</v>
+      </c>
+      <c r="AT2">
+        <v>46</v>
+      </c>
+      <c r="AU2">
+        <v>47</v>
+      </c>
+      <c r="AV2">
+        <v>48</v>
+      </c>
+      <c r="AW2">
+        <v>49</v>
+      </c>
+      <c r="AX2">
+        <v>50</v>
+      </c>
+      <c r="AY2">
+        <v>51</v>
+      </c>
+      <c r="AZ2">
+        <v>52</v>
+      </c>
+      <c r="BA2">
+        <v>53</v>
+      </c>
+      <c r="BB2">
+        <v>54</v>
+      </c>
+      <c r="BC2">
+        <v>55</v>
+      </c>
+      <c r="BD2">
+        <v>56</v>
+      </c>
+      <c r="BE2">
+        <v>57</v>
+      </c>
+      <c r="BF2">
+        <v>58</v>
+      </c>
+      <c r="BG2">
+        <v>59</v>
+      </c>
+      <c r="BH2">
+        <v>60</v>
+      </c>
+      <c r="BI2">
+        <v>61</v>
+      </c>
+      <c r="BJ2">
+        <v>62</v>
+      </c>
+      <c r="BK2">
+        <v>63</v>
+      </c>
+      <c r="BL2">
+        <v>64</v>
+      </c>
+      <c r="BM2">
+        <v>65</v>
+      </c>
+      <c r="BN2">
+        <v>66</v>
+      </c>
+      <c r="BO2">
+        <v>67</v>
+      </c>
+      <c r="BP2">
+        <v>68</v>
+      </c>
+      <c r="BQ2">
+        <v>69</v>
+      </c>
+      <c r="BR2">
+        <v>70</v>
+      </c>
+      <c r="BS2">
+        <v>71</v>
+      </c>
+      <c r="BT2">
+        <v>72</v>
+      </c>
+      <c r="BU2">
+        <v>73</v>
+      </c>
+      <c r="BV2">
+        <v>74</v>
+      </c>
+      <c r="BW2">
+        <v>75</v>
+      </c>
+      <c r="BX2">
+        <v>76</v>
+      </c>
+      <c r="BY2">
+        <v>77</v>
+      </c>
+      <c r="BZ2">
+        <v>78</v>
+      </c>
+      <c r="CA2">
+        <v>79</v>
+      </c>
+      <c r="CB2">
+        <v>80</v>
+      </c>
+      <c r="CC2">
+        <v>81</v>
+      </c>
+      <c r="CD2">
+        <v>82</v>
+      </c>
+      <c r="CE2">
+        <v>83</v>
+      </c>
+      <c r="CF2">
+        <v>84</v>
+      </c>
+      <c r="CG2">
+        <v>85</v>
+      </c>
+      <c r="CH2">
+        <v>86</v>
+      </c>
+      <c r="CI2">
+        <v>87</v>
+      </c>
+      <c r="CJ2">
+        <v>88</v>
+      </c>
+      <c r="CK2">
+        <v>89</v>
+      </c>
+      <c r="CL2">
+        <v>90</v>
+      </c>
+      <c r="CM2">
+        <v>91</v>
+      </c>
+      <c r="CN2">
+        <v>92</v>
+      </c>
+      <c r="CO2">
+        <v>93</v>
+      </c>
+      <c r="CP2">
+        <v>94</v>
+      </c>
+      <c r="CQ2">
+        <v>95</v>
+      </c>
+      <c r="CR2">
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>